<commit_message>
Create header with bootstrap jumbotron and a placeholder for outputting the winning message.  Update the style.css with black for the body and jumbotron
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6408732A-9BB2-4462-83D5-AF54A2A76FAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A5E184-C2E4-418A-BBBA-4EB51FBF1847}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="948" yWindow="0" windowWidth="20382" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>I want a header at the top that display an 80's logo</t>
   </si>
@@ -81,6 +80,9 @@
   <si>
     <t>Background black
 start with a picture of a old school hangman game</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -407,7 +409,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -445,7 +447,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B10" si="0">ROW()-1</f>
         <v>2</v>

</xml_diff>

<commit_message>
Used a bootstrap alert tag in the jumbotron instead of a h1 tag.  Create a 2 column boostrap grid for the content of the game.  Add hangman image in left column.  Add the text for the game in the right column
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A5E184-C2E4-418A-BBBA-4EB51FBF1847}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12343EB-F344-4F62-970B-3119A11029A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="948" yWindow="0" windowWidth="20382" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>I want a header at the top that display an 80's logo</t>
   </si>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -434,7 +434,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B2" s="1">
         <f>ROW()-1</f>
         <v>1</v>

</xml_diff>

<commit_message>
add javascript to intake a letter, check that the letter is in the alphabet only, ignore duplicates, updated [letters guessed] div, and update the botstrap alert to say game is started
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12343EB-F344-4F62-970B-3119A11029A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AEA4D3-05EE-4CC4-A729-53F2FADED888}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="948" yWindow="0" windowWidth="20382" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>I want a header at the top that display an 80's logo</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -510,7 +513,9 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>

</xml_diff>

<commit_message>
same as last commit
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AEA4D3-05EE-4CC4-A729-53F2FADED888}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B10B3C3-ACA5-4B53-9124-41CEB6BCB0AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="948" yWindow="0" windowWidth="20382" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>I want a header at the top that display an 80's logo</t>
   </si>
@@ -85,7 +85,13 @@
     <t>x</t>
   </si>
   <si>
-    <t>in progress</t>
+    <t>alphabets only, no duplicates</t>
+  </si>
+  <si>
+    <t>Restart game on failure</t>
+  </si>
+  <si>
+    <t>When game ends restart the game when user</t>
   </si>
 </sst>
 </file>
@@ -409,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -514,7 +520,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
@@ -523,7 +529,9 @@
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1"/>
@@ -548,6 +556,14 @@
         <v>13</v>
       </c>
       <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added javascript to change image when user loses to loser.jpg
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B10B3C3-ACA5-4B53-9124-41CEB6BCB0AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ED5DA2-74BA-4733-A6F8-D8C26B8F0568}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="0" windowWidth="20382" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="2010" windowWidth="20898" windowHeight="9684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>I want a header at the top that display an 80's logo</t>
   </si>
@@ -64,18 +64,10 @@
     <t>Image provided</t>
   </si>
   <si>
-    <t>after user starts the "press any key" should disappear and replaced with "start time"</t>
-  </si>
-  <si>
     <t>If the users exceeds the amount of guesses then game should end and displayed a 80's funny image instead of a band/singer.</t>
   </si>
   <si>
     <t xml:space="preserve">When the user wins </t>
-  </si>
-  <si>
-    <t>display the image of the band or singer in the left panel.
-Diplay a song from the band/singer on the top of the grid
-Play the song (audio)</t>
   </si>
   <si>
     <t>Background black
@@ -91,7 +83,20 @@
     <t>Restart game on failure</t>
   </si>
   <si>
-    <t>When game ends restart the game when user</t>
+    <t>Display pop-up alerting user the game is over
+Update the banner with a message that says game is over press any key to start another. 
+Change the color of the banner to red.
+Reset the letters guessed and remaining guesses.</t>
+  </si>
+  <si>
+    <t>Game starts when any key is pressed.
+Banner message color (amber) and message is changed to notify the user the the game started.</t>
+  </si>
+  <si>
+    <t>display the image of the band or singer in the left panel.
+Diplay a song from the band/singer on the top banner.
+Change the banner color to green
+Play the song (audio)</t>
   </si>
 </sst>
 </file>
@@ -127,13 +132,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -444,7 +452,7 @@
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <f>ROW()-1</f>
@@ -454,12 +462,12 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B10" si="0">ROW()-1</f>
@@ -472,8 +480,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -481,8 +491,8 @@
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -508,7 +518,9 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -520,7 +532,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
@@ -530,20 +542,20 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -553,16 +565,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added readme.md file with pseudocode
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ED5DA2-74BA-4733-A6F8-D8C26B8F0568}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6662D187-BA6F-452C-A2F8-6990B27F3C1E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2010" windowWidth="20898" windowHeight="9684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19335" yWindow="-14205" windowWidth="18945" windowHeight="10185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>I want a header at the top that display an 80's logo</t>
   </si>
@@ -425,9 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -496,7 +494,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -507,7 +507,9 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -546,7 +548,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -559,7 +563,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -570,6 +576,9 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>